<commit_message>
Corrected the PCBWAY BOM
</commit_message>
<xml_diff>
--- a/pcb/sensors/Open_Telemetry_digitalSensorShield/Manufacturing/W32271ASH4-5sets-Open_Telemetry_digitalSensorShieldBOM_PCBWay.xlsx
+++ b/pcb/sensors/Open_Telemetry_digitalSensorShield/Manufacturing/W32271ASH4-5sets-Open_Telemetry_digitalSensorShieldBOM_PCBWay.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Projects\open_telemetry_HW\pcb\sensors\Open_Telemetry_digitalSensorShield\Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{E3AADF3C-D13E-4532-A84D-84CF7FAC70BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4F885E0B-A428-4E84-A4DF-EAA5685FEA5C}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{E3AADF3C-D13E-4532-A84D-84CF7FAC70BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0C62EB58-22CF-4AAD-B6D0-7CD2C764B2D7}"/>
   <bookViews>
     <workbookView xWindow="2655" yWindow="555" windowWidth="23400" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>package:0201</t>
-  </si>
-  <si>
-    <t>R2, R6</t>
   </si>
   <si>
     <t>RC0201JR-071KL</t>
@@ -504,7 +501,10 @@
     <t>R1, R8, R9, R15, R16, R17, R18</t>
   </si>
   <si>
-    <t>R3, R5, R19, R20</t>
+    <t>R2, R6, R19, R20</t>
+  </si>
+  <si>
+    <t>R3, R5</t>
   </si>
 </sst>
 </file>
@@ -515,12 +515,19 @@
     <numFmt numFmtId="164" formatCode="\$#,##0.000_);[Red]\(\$#,##0.000\)"/>
     <numFmt numFmtId="165" formatCode="\$#,##0;\-\$#,##0"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -660,7 +667,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -669,56 +676,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
@@ -1175,7 +1182,7 @@
   <dimension ref="A2:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1195,25 +1202,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="19.5" customHeight="1">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="D2" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="D2" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:13">
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
     </row>
     <row r="6" spans="1:13" ht="28.5" customHeight="1">
       <c r="A6" s="4" t="s">
@@ -1672,8 +1679,8 @@
       <c r="A18" s="5">
         <v>12</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>122</v>
+      <c r="B18" s="20" t="s">
+        <v>121</v>
       </c>
       <c r="C18" s="5">
         <v>7</v>
@@ -1688,7 +1695,7 @@
         <v>78</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>18</v>
@@ -1713,36 +1720,36 @@
         <v>13</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>81</v>
+        <v>122</v>
       </c>
       <c r="C19" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>76</v>
       </c>
       <c r="E19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="G19" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K19" s="15">
         <v>1.2E-2</v>
       </c>
       <c r="L19" s="15">
         <f t="shared" si="0"/>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
       <c r="M19" s="16" t="s">
         <v>80</v>
@@ -1752,37 +1759,37 @@
       <c r="A20" s="5">
         <v>14</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="24" t="s">
         <v>123</v>
       </c>
       <c r="C20" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>76</v>
       </c>
       <c r="E20" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="G20" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K20" s="15">
         <v>1.2E-2</v>
       </c>
       <c r="L20" s="15">
         <f t="shared" si="0"/>
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
       <c r="M20" s="16" t="s">
         <v>80</v>
@@ -1793,7 +1800,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="5">
         <v>4</v>
@@ -1802,10 +1809,10 @@
         <v>76</v>
       </c>
       <c r="E21" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>23</v>
@@ -1815,7 +1822,7 @@
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K21" s="15">
         <v>1.2E-2</v>
@@ -1825,7 +1832,7 @@
         <v>0.24</v>
       </c>
       <c r="M21" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15">
@@ -1833,19 +1840,19 @@
         <v>16</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C22" s="5">
         <v>1</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>23</v>
@@ -1855,7 +1862,7 @@
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K22" s="15">
         <v>0.1</v>
@@ -1865,7 +1872,7 @@
         <v>0.5</v>
       </c>
       <c r="M22" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15">
@@ -1873,19 +1880,19 @@
         <v>17</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C23" s="5">
         <v>2</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="F23" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>39</v>
@@ -1897,7 +1904,7 @@
         <v>40</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K23" s="15">
         <v>0.54200000000000004</v>
@@ -1912,29 +1919,29 @@
         <v>18</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" s="5">
         <v>1</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="G24" s="6" t="s">
         <v>106</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="H24" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K24" s="15">
         <v>3.6</v>
@@ -1949,29 +1956,29 @@
         <v>19</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25" s="5">
         <v>1</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="G25" s="11" t="s">
         <v>112</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>113</v>
       </c>
       <c r="H25" s="11" t="s">
         <v>18</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K25" s="15">
         <v>5.867</v>
@@ -1986,7 +1993,7 @@
         <v>20</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C26" s="12">
         <v>2</v>
@@ -1995,27 +2002,27 @@
         <v>76</v>
       </c>
       <c r="E26" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="F26" s="12" t="s">
-        <v>117</v>
-      </c>
       <c r="G26" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H26" s="13" t="s">
         <v>18</v>
       </c>
       <c r="I26" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="J26" s="14" t="s">
         <v>118</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>119</v>
       </c>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
       <c r="M26" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N26" s="18"/>
       <c r="O26" s="18"/>

</xml_diff>